<commit_message>
created auto-picklisting tab with slider, download option, and other things. need to change table aesthetics? not sure
</commit_message>
<xml_diff>
--- a/Shiny App Files/data files/Severn/severnPicklist.xlsx
+++ b/Shiny App Files/data files/Severn/severnPicklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shriy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shriy\scouting2025\Shiny App Files\data files\Severn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B20C70-0F23-4CA0-874F-101D49C85982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB03E097-92A9-48E5-95B8-375B68389102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="120">
   <si>
     <t>Merged</t>
   </si>
@@ -58,9 +58,6 @@
     <t>&lt;-- fixed connectivity issues?</t>
   </si>
   <si>
-    <t>they have a similar weight robot as 623 with half the height; think they should be over 623</t>
-  </si>
-  <si>
     <t>Best</t>
   </si>
   <si>
@@ -395,13 +392,19 @@
   </si>
   <si>
     <t>"they don't know the rules"</t>
+  </si>
+  <si>
+    <t>339?</t>
+  </si>
+  <si>
+    <t>623; INSANE defense</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -462,8 +465,16 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,6 +569,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
   </fills>
@@ -758,7 +775,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -853,6 +870,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1112,17 +1133,18 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="73.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1131,35 +1153,35 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="2">
+      <c r="A2" s="60">
         <v>2106</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A3" s="2">
+      <c r="A3" s="60">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A4" s="60">
         <v>888</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A4" s="2">
-        <v>1727</v>
-      </c>
-    </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A5" s="3">
+      <c r="A5" s="62">
         <v>2199</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A6" s="3">
+      <c r="A6" s="62">
         <v>10224</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="3">
+    <row r="7" spans="1:8" ht="13">
+      <c r="A7" s="62">
         <v>3748</v>
       </c>
       <c r="C7" s="4">
@@ -1172,8 +1194,8 @@
         <v>3793</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="3">
+    <row r="8" spans="1:8" ht="13">
+      <c r="A8" s="62">
         <v>4541</v>
       </c>
       <c r="C8" s="7">
@@ -1189,8 +1211,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3">
+    <row r="9" spans="1:8" ht="13">
+      <c r="A9" s="62">
         <v>1811</v>
       </c>
       <c r="C9" s="8">
@@ -1209,8 +1231,8 @@
         <v>3714</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="3">
+    <row r="10" spans="1:8" ht="13">
+      <c r="A10" s="62">
         <v>1111</v>
       </c>
       <c r="C10" s="7">
@@ -1223,8 +1245,8 @@
         <v>10449</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="3">
+    <row r="11" spans="1:8" ht="13">
+      <c r="A11" s="61">
         <v>1885</v>
       </c>
       <c r="C11" s="7">
@@ -1235,8 +1257,8 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="3">
+    <row r="12" spans="1:8" ht="13">
+      <c r="A12" s="62">
         <v>404</v>
       </c>
       <c r="C12" s="5">
@@ -1246,9 +1268,9 @@
         <v>9709</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="10">
-        <v>2377</v>
+    <row r="13" spans="1:8" ht="13">
+      <c r="A13" s="63" t="s">
+        <v>119</v>
       </c>
       <c r="C13" s="11">
         <v>10679</v>
@@ -1258,52 +1280,49 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A14" s="10">
+      <c r="A14" s="63" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A15" s="63">
+        <v>2377</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A16" s="63">
         <v>8622</v>
       </c>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A15" s="10">
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1">
+      <c r="B17" s="63">
         <v>5587</v>
-      </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A16" s="10">
-        <v>3793</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A17" s="10">
-        <v>7886</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1">
       <c r="A18" s="10">
+        <v>3793</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A19" s="63">
+        <v>7886</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="12.5">
+      <c r="A20" s="63">
         <v>9403</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A19" s="10">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="12.5">
-      <c r="A20" s="10">
-        <v>623</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" ht="12.5">
-      <c r="A21" s="10">
+      <c r="A21" s="63">
         <v>7770</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.5">
-      <c r="A22" s="10">
+      <c r="A22" s="63">
         <v>2421</v>
       </c>
     </row>
@@ -1313,7 +1332,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="12.5">
-      <c r="A24" s="10">
+      <c r="A24" s="63">
         <v>2537</v>
       </c>
     </row>
@@ -1323,13 +1342,11 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="12.5">
-      <c r="A26" s="10">
+      <c r="A26" s="63">
         <v>10679</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="12.5">
-      <c r="A27" s="2"/>
-    </row>
+    <row r="27" spans="1:2" ht="12.5"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1342,62 +1359,64 @@
   </sheetPr>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" ht="13">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="J1" s="12"/>
       <c r="K1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="O1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="S1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="T1" s="16" t="s">
         <v>20</v>
-      </c>
-      <c r="T1" s="16" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15.75" customHeight="1">
@@ -1420,7 +1439,7 @@
         <v>3714</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="18">
@@ -1452,7 +1471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" ht="13">
       <c r="A3" s="2">
         <v>2106</v>
       </c>
@@ -1501,7 +1520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" ht="13">
       <c r="A4" s="2">
         <v>888</v>
       </c>
@@ -1544,7 +1563,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" ht="13">
       <c r="A5" s="2">
         <v>1727</v>
       </c>
@@ -1587,7 +1606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" ht="13">
       <c r="B6" s="3">
         <v>1811</v>
       </c>
@@ -1598,7 +1617,7 @@
         <v>8622</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J6" s="24"/>
       <c r="K6" s="18">
@@ -1630,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" ht="13">
       <c r="B7" s="3">
         <v>1111</v>
       </c>
@@ -1644,7 +1663,7 @@
         <v>404</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J7" s="24"/>
       <c r="K7" s="18">
@@ -1676,7 +1695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" ht="13">
       <c r="B8" s="3">
         <v>1885</v>
       </c>
@@ -1690,7 +1709,7 @@
         <v>1885</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J8" s="24"/>
       <c r="K8" s="18">
@@ -1722,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" ht="13">
       <c r="B9" s="3">
         <v>404</v>
       </c>
@@ -1762,7 +1781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" ht="13">
       <c r="C10" s="2">
         <v>2421</v>
       </c>
@@ -1799,9 +1818,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" ht="13">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2">
         <v>4464</v>
@@ -1810,7 +1829,7 @@
         <v>3714</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J11" s="24"/>
       <c r="K11" s="18">
@@ -1842,9 +1861,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" ht="13">
       <c r="A12" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2">
         <v>7886</v>
@@ -1885,9 +1904,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" ht="13">
       <c r="A13" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2">
         <v>10449</v>
@@ -1928,7 +1947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" ht="13">
       <c r="C14" s="2">
         <v>9709</v>
       </c>
@@ -1968,7 +1987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" ht="13">
       <c r="C15" s="2">
         <v>623</v>
       </c>
@@ -2008,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" ht="13">
       <c r="C16" s="2">
         <v>5587</v>
       </c>
@@ -2045,7 +2064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" ht="13">
       <c r="C17" s="2">
         <v>3714</v>
       </c>
@@ -2082,7 +2101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" ht="13">
       <c r="J18" s="24"/>
       <c r="K18" s="18">
         <v>3793</v>
@@ -2113,9 +2132,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" ht="13">
       <c r="A19" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="31"/>
       <c r="C19" s="32"/>
@@ -2151,7 +2170,7 @@
     </row>
     <row r="20" spans="1:20" ht="13">
       <c r="A20" s="51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="52"/>
       <c r="C20" s="53"/>
@@ -2255,7 +2274,7 @@
     </row>
     <row r="23" spans="1:20" ht="13">
       <c r="A23" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="31"/>
       <c r="C23" s="32"/>
@@ -2291,7 +2310,7 @@
     </row>
     <row r="24" spans="1:20" ht="13">
       <c r="A24" s="51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="52"/>
       <c r="C24" s="53"/>
@@ -2361,7 +2380,7 @@
     </row>
     <row r="26" spans="1:20" ht="13">
       <c r="A26" s="51" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="52"/>
       <c r="C26" s="53"/>
@@ -2400,7 +2419,7 @@
       <c r="B27" s="58"/>
       <c r="C27" s="59"/>
       <c r="D27" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J27" s="24"/>
       <c r="K27" s="18">
@@ -2434,7 +2453,7 @@
     </row>
     <row r="28" spans="1:20" ht="13">
       <c r="D28" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" s="24"/>
       <c r="K28" s="18">
@@ -2589,7 +2608,7 @@
         <v>2377</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" customHeight="1">
@@ -2597,7 +2616,7 @@
         <v>8622</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1">
@@ -2605,7 +2624,7 @@
         <v>3793</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" customHeight="1">
@@ -2613,12 +2632,12 @@
         <v>4464</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" customHeight="1">
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2640,50 +2659,50 @@
     <col min="10" max="10" width="23.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="13">
       <c r="A1" s="42"/>
       <c r="B1" s="43"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="13">
       <c r="A2" s="42"/>
       <c r="B2" s="43"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" ht="13">
       <c r="A3" s="42"/>
       <c r="B3" s="43"/>
       <c r="G3" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="13">
       <c r="A4" s="9"/>
       <c r="B4" s="43"/>
       <c r="C4" s="3">
         <v>2537</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+    </row>
+    <row r="5" spans="1:12" ht="13">
       <c r="A5" s="43">
         <v>1</v>
       </c>
@@ -2691,10 +2710,10 @@
         <v>339</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="13">
       <c r="A6" s="43">
         <v>2</v>
       </c>
@@ -2702,10 +2721,10 @@
         <v>2537</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="13">
       <c r="A7" s="43">
         <v>3</v>
       </c>
@@ -2713,10 +2732,10 @@
         <v>10679</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="13">
       <c r="A8" s="43" t="s">
         <v>3</v>
       </c>
@@ -2724,33 +2743,33 @@
         <v>3714</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="J8" s="2">
         <v>3714</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="K9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1">
@@ -2758,30 +2777,30 @@
         <v>3714</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="D11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
@@ -2789,15 +2808,15 @@
         <v>2537</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="I14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1">
@@ -2805,7 +2824,7 @@
         <v>10679</v>
       </c>
       <c r="K16" s="44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="3:12" ht="15.75" customHeight="1">
@@ -2813,27 +2832,27 @@
         <v>339</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="2">
         <v>2.25</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="18" spans="3:12" ht="15.75" customHeight="1">
       <c r="K18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="23" spans="3:12" ht="12.5">
@@ -2841,13 +2860,13 @@
         <v>10679</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2871,35 +2890,35 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
       <c r="A1" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="C1" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="D1" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="E1" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="F1" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="G1" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="H1" s="46" t="s">
         <v>84</v>
-      </c>
-      <c r="H1" s="46" t="s">
-        <v>85</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="47" t="s">
         <v>86</v>
-      </c>
-      <c r="K1" s="47" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
@@ -2913,10 +2932,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="H2" s="2">
         <v>0.12</v>
@@ -2925,7 +2944,7 @@
         <v>113</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
@@ -2939,13 +2958,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="H3" s="2">
         <v>2.87</v>
@@ -2959,13 +2978,13 @@
         <v>2.25</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="H4" s="2">
         <v>3.36</v>
@@ -2974,7 +2993,7 @@
         <v>100</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
@@ -2988,16 +3007,16 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" s="2">
         <v>3.38</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
@@ -3011,13 +3030,13 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="H6" s="2">
         <v>1.62</v>
@@ -3026,7 +3045,7 @@
         <v>113</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
@@ -3040,10 +3059,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H7" s="2">
         <v>2.87</v>
@@ -3057,7 +3076,7 @@
         <v>2.11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H8" s="2">
         <v>3.56</v>
@@ -3068,13 +3087,13 @@
         <v>3714</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3098,25 +3117,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
@@ -3159,7 +3178,7 @@
         <v>0.88</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
@@ -3202,7 +3221,7 @@
         <v>0.12</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
@@ -3210,22 +3229,22 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" s="2">
         <v>2377</v>
@@ -3239,7 +3258,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" s="2">
         <v>7886</v>
@@ -3264,7 +3283,7 @@
         <v>10449</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>